<commit_message>
ajout du calcul auto de la regression des courbes moteurs.
</commit_message>
<xml_diff>
--- a/Analyses/Courbes_Moteurs.xlsx
+++ b/Analyses/Courbes_Moteurs.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="8910" windowHeight="1170" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="8910" windowHeight="1170"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">Feuil1!$D$58</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Feuil1!$D$67</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
@@ -21,7 +21,7 @@
     <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Feuil1!$D$61</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Feuil1!$D$70</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
@@ -30,12 +30,12 @@
     <definedName name="solver_typ" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="124">
   <si>
     <t>Masse linéique de la barre de soutien</t>
   </si>
@@ -401,13 +401,19 @@
   </si>
   <si>
     <t>M76</t>
+  </si>
+  <si>
+    <t>Pente</t>
+  </si>
+  <si>
+    <t>Origine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="15">
     <numFmt numFmtId="164" formatCode="0.00\ \g\/\m"/>
     <numFmt numFmtId="165" formatCode="0.00\ \m"/>
     <numFmt numFmtId="166" formatCode="0.00\ \m\/\s\²"/>
@@ -419,8 +425,12 @@
     <numFmt numFmtId="172" formatCode="0.000\ \N"/>
     <numFmt numFmtId="173" formatCode="0\ \k\m"/>
     <numFmt numFmtId="174" formatCode="0.0"/>
+    <numFmt numFmtId="175" formatCode="0.00&quot; A/u&quot;"/>
+    <numFmt numFmtId="176" formatCode="0.00&quot; N/u&quot;"/>
+    <numFmt numFmtId="177" formatCode="0.000&quot; A/u&quot;"/>
+    <numFmt numFmtId="178" formatCode="0.000&quot; N/u&quot;"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -472,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -531,19 +541,48 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
-  <c:style val="41"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="141"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="41"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
@@ -551,6 +590,7 @@
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -644,6 +684,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -673,7 +714,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$C$31:$C$40</c:f>
+              <c:f>Feuil1!$C$34:$C$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -712,7 +753,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$H$31:$H$40</c:f>
+              <c:f>Feuil1!$H$34:$H$43</c:f>
               <c:numCache>
                 <c:formatCode>0.000\ \N</c:formatCode>
                 <c:ptCount val="10"/>
@@ -749,6 +790,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -787,10 +829,12 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$C$43:$C$52</c:f>
+              <c:f>Feuil1!$C$49:$C$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -829,7 +873,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$H$43:$H$52</c:f>
+              <c:f>Feuil1!$H$49:$H$58</c:f>
               <c:numCache>
                 <c:formatCode>0.000\ \N</c:formatCode>
                 <c:ptCount val="10"/>
@@ -866,17 +910,27 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="121207424"/>
-        <c:axId val="121225984"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="250555688"/>
+        <c:axId val="329040976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121207424"/>
+        <c:axId val="250555688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1750"/>
           <c:min val="1200"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:minorGridlines/>
@@ -897,18 +951,22 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121225984"/>
+        <c:crossAx val="329040976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121225984"/>
+        <c:axId val="329040976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:minorGridlines/>
@@ -929,10 +987,13 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.000\ \N" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121207424"/>
+        <c:crossAx val="250555688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -940,8 +1001,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -953,8 +1017,17 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
-  <c:style val="41"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="141"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="41"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
@@ -962,6 +1035,7 @@
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1055,6 +1129,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1084,7 +1159,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$H$31:$H$40</c:f>
+              <c:f>Feuil1!$H$34:$H$43</c:f>
               <c:numCache>
                 <c:formatCode>0.000\ \N</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1123,7 +1198,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$E$31:$E$40</c:f>
+              <c:f>Feuil1!$E$34:$E$43</c:f>
               <c:numCache>
                 <c:formatCode>0.00\ \A</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1160,6 +1235,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1186,7 +1262,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$H$43:$H$52</c:f>
+              <c:f>Feuil1!$H$49:$H$58</c:f>
               <c:numCache>
                 <c:formatCode>0.000\ \N</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1225,7 +1301,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$E$43:$E$52</c:f>
+              <c:f>Feuil1!$E$49:$E$58</c:f>
               <c:numCache>
                 <c:formatCode>0.00\ \A</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1262,15 +1338,25 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="121263616"/>
-        <c:axId val="121290752"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="329044504"/>
+        <c:axId val="329043720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121263616"/>
+        <c:axId val="329044504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:minorGridlines/>
@@ -1291,18 +1377,22 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.000\ \N" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121290752"/>
+        <c:crossAx val="329043720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121290752"/>
+        <c:axId val="329043720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:minorGridlines/>
@@ -1323,10 +1413,13 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00\ \A" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121263616"/>
+        <c:crossAx val="329044504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1334,8 +1427,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1347,8 +1443,17 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
-  <c:style val="41"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="141"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="41"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
@@ -1356,6 +1461,7 @@
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1437,6 +1543,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1466,7 +1573,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$E$31:$E$40</c:f>
+              <c:f>Feuil1!$E$34:$E$43</c:f>
               <c:numCache>
                 <c:formatCode>0.00\ \A</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1505,7 +1612,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$C$31:$C$40</c:f>
+              <c:f>Feuil1!$C$34:$C$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1542,6 +1649,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1568,6 +1676,7 @@
           </c:marker>
           <c:trendline>
             <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout/>
@@ -1576,7 +1685,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$E$43:$E$53</c:f>
+              <c:f>Feuil1!$E$49:$E$59</c:f>
               <c:numCache>
                 <c:formatCode>0.00\ \A</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1615,7 +1724,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$C$43:$C$53</c:f>
+              <c:f>Feuil1!$C$49:$C$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1652,17 +1761,27 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="131457792"/>
-        <c:axId val="131460096"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="329042936"/>
+        <c:axId val="329041760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="131457792"/>
+        <c:axId val="329042936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12"/>
           <c:min val="0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:minorGridlines/>
@@ -1683,19 +1802,23 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00\ \A" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131460096"/>
+        <c:crossAx val="329041760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="131460096"/>
+        <c:axId val="329041760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1200"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:minorGridlines/>
@@ -1716,10 +1839,13 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131457792"/>
+        <c:crossAx val="329042936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1727,8 +1853,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1740,8 +1869,17 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
-  <c:style val="41"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="141"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="41"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
@@ -1749,6 +1887,7 @@
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2246,15 +2385,25 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="116930432"/>
-        <c:axId val="118235136"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="329042544"/>
+        <c:axId val="327290080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="116930432"/>
+        <c:axId val="329042544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:minorGridlines/>
@@ -2275,18 +2424,22 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118235136"/>
+        <c:crossAx val="327290080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="118235136"/>
+        <c:axId val="327290080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:minorGridlines/>
@@ -2307,15 +2460,20 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116930432"/>
+        <c:crossAx val="329042544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2337,7 +2495,7 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>142874</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2361,13 +2519,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2391,13 +2549,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>88</xdr:row>
       <xdr:rowOff>76201</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2498,7 +2656,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2530,9 +2688,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2564,6 +2723,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3855,14 +4015,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:K67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:K76"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
@@ -3870,7 +4030,7 @@
     <col min="9" max="11" width="11.42578125" style="17"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
@@ -3878,7 +4038,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="3:7">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
@@ -3886,7 +4046,7 @@
         <v>0.95799999999999996</v>
       </c>
     </row>
-    <row r="5" spans="3:7">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
@@ -3894,7 +4054,7 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="6" spans="3:7">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3902,7 +4062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="3:7">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
@@ -3910,7 +4070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="3:7">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
@@ -3918,7 +4078,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="9" spans="3:7">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
@@ -3926,11 +4086,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="3:7">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="3:7">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>4</v>
       </c>
@@ -3939,7 +4099,7 @@
         <v>257.72586326122467</v>
       </c>
     </row>
-    <row r="12" spans="3:7">
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>5</v>
       </c>
@@ -3948,7 +4108,7 @@
         <v>0.66065365948688293</v>
       </c>
     </row>
-    <row r="13" spans="3:7">
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
         <v>9</v>
       </c>
@@ -3957,10 +4117,10 @@
         <v>63.290620578843388</v>
       </c>
     </row>
-    <row r="14" spans="3:7">
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G14" s="7"/>
     </row>
-    <row r="16" spans="3:7">
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
@@ -3968,7 +4128,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="15" customHeight="1">
+    <row r="18" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="21" t="s">
         <v>30</v>
       </c>
@@ -4000,7 +4160,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="2:11">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="21"/>
       <c r="C19" s="7">
         <v>1230</v>
@@ -4033,7 +4193,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="2:11">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="21"/>
       <c r="C20" s="7">
         <v>1305</v>
@@ -4069,7 +4229,7 @@
         <v>1.7265569979254687</v>
       </c>
     </row>
-    <row r="21" spans="2:11">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="21"/>
       <c r="C21" s="7">
         <v>1410</v>
@@ -4105,7 +4265,7 @@
         <v>2.8974404792772233</v>
       </c>
     </row>
-    <row r="22" spans="2:11">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="21"/>
       <c r="C22" s="7">
         <v>1480</v>
@@ -4141,7 +4301,7 @@
         <v>4.9018342354895479</v>
       </c>
     </row>
-    <row r="23" spans="2:11">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="21"/>
       <c r="C23" s="7">
         <v>1580</v>
@@ -4177,7 +4337,7 @@
         <v>3.572186892259591</v>
       </c>
     </row>
-    <row r="24" spans="2:11">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="21"/>
       <c r="C24" s="7">
         <v>1665</v>
@@ -4213,7 +4373,7 @@
         <v>3.9690965469550981</v>
       </c>
     </row>
-    <row r="25" spans="2:11">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="21"/>
       <c r="C25" s="7"/>
       <c r="D25" s="6">
@@ -4245,7 +4405,7 @@
         <v>-17.067115151906936</v>
       </c>
     </row>
-    <row r="26" spans="2:11">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="21"/>
       <c r="C26" s="7"/>
       <c r="D26" s="6">
@@ -4277,7 +4437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:11">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="21"/>
       <c r="C27" s="7"/>
       <c r="D27" s="6">
@@ -4309,7 +4469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:11">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="21"/>
       <c r="C28" s="7"/>
       <c r="D28" s="6">
@@ -4341,951 +4501,1059 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:11">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="2:11" ht="15" customHeight="1">
-      <c r="B30" s="21" t="s">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30">
+        <f>SLOPE(C19:C28,H19:H28)</f>
+        <v>174.07323427360225</v>
+      </c>
+      <c r="E30" s="24">
+        <f>SLOPE(E19:E28,C19:C28)</f>
+        <v>2.0368050407709413E-2</v>
+      </c>
+      <c r="H30" s="25">
+        <f>SLOPE(H19:H28,C19:C28)</f>
+        <v>5.7336973166759843E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31">
+        <f>INTERCEPT(C19:C28,H19:H28)</f>
+        <v>1225.7142857142858</v>
+      </c>
+      <c r="E31" s="22">
+        <f>INTERCEPT(E19:E28,C19:C28)</f>
+        <v>-25.565166172473436</v>
+      </c>
+      <c r="H31" s="23">
+        <f>INTERCEPT(H19:H28,C19:C28)</f>
+        <v>-7.0254601013922535</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="H33" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I30" s="18" t="s">
+      <c r="I33" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="J30" s="18" t="s">
+      <c r="J33" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="K30" s="18" t="s">
+      <c r="K33" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="2:11">
-      <c r="B31" s="21"/>
-      <c r="C31" s="7">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B34" s="21"/>
+      <c r="C34" s="7">
         <v>1230</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D34" s="6">
         <v>1000</v>
       </c>
-      <c r="E31" s="10">
+      <c r="E34" s="10">
         <v>0</v>
       </c>
-      <c r="F31" s="6">
-        <f>$D$16-D31</f>
+      <c r="F34" s="6">
+        <f>$D$16-D34</f>
         <v>0</v>
       </c>
-      <c r="G31" s="6">
-        <f>F31*(1-$G$12)/$G$12</f>
+      <c r="G34" s="6">
+        <f>F34*(1-$G$12)/$G$12</f>
         <v>0</v>
       </c>
-      <c r="H31" s="11">
-        <f>G31*$G$5/1000</f>
+      <c r="H34" s="11">
+        <f>G34*$G$5/1000</f>
         <v>0</v>
       </c>
-      <c r="I31" s="19" t="s">
+      <c r="I34" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="J31" s="19" t="s">
+      <c r="J34" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="K31" s="19" t="s">
+      <c r="K34" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="2:11">
-      <c r="B32" s="21"/>
-      <c r="C32" s="7">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B35" s="21"/>
+      <c r="C35" s="7">
         <v>1280</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D35" s="6">
         <v>900</v>
       </c>
-      <c r="E32" s="10">
+      <c r="E35" s="10">
         <v>0.6</v>
       </c>
-      <c r="F32" s="6">
-        <f t="shared" ref="F32:F33" si="8">$D$16-D32</f>
+      <c r="F35" s="6">
+        <f t="shared" ref="F35:F36" si="8">$D$16-D35</f>
         <v>100</v>
       </c>
-      <c r="G32" s="6">
-        <f t="shared" ref="G32:G33" si="9">F32*(1-$G$12)/$G$12</f>
+      <c r="G35" s="6">
+        <f t="shared" ref="G35:G36" si="9">F35*(1-$G$12)/$G$12</f>
         <v>51.365240416087431</v>
       </c>
-      <c r="H32" s="11">
-        <f t="shared" ref="H32:H40" si="10">G32*$G$5/1000</f>
+      <c r="H35" s="11">
+        <f t="shared" ref="H35:H43" si="10">G35*$G$5/1000</f>
         <v>0.50389300848181773</v>
       </c>
-      <c r="I32" s="20">
-        <f>C32-C31</f>
+      <c r="I35" s="20">
+        <f>C35-C34</f>
         <v>50</v>
       </c>
-      <c r="J32" s="20">
-        <f>(C32-C31)/(H32-H31)</f>
+      <c r="J35" s="20">
+        <f>(C35-C34)/(H35-H34)</f>
         <v>99.227413673877521</v>
       </c>
-      <c r="K32" s="20">
-        <f>(E32-E31)/(H32-H31)</f>
+      <c r="K35" s="20">
+        <f>(E35-E34)/(H35-H34)</f>
         <v>1.1907289640865302</v>
       </c>
     </row>
-    <row r="33" spans="2:11">
-      <c r="B33" s="21"/>
-      <c r="C33" s="7">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B36" s="21"/>
+      <c r="C36" s="7">
         <v>1335</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D36" s="6">
         <v>800</v>
       </c>
-      <c r="E33" s="10">
+      <c r="E36" s="10">
         <v>1.53</v>
       </c>
-      <c r="F33" s="6">
+      <c r="F36" s="6">
         <f t="shared" si="8"/>
         <v>200</v>
       </c>
-      <c r="G33" s="6">
+      <c r="G36" s="6">
         <f t="shared" si="9"/>
         <v>102.73048083217486</v>
       </c>
-      <c r="H33" s="11">
+      <c r="H36" s="11">
         <f t="shared" si="10"/>
         <v>1.0077860169636355</v>
       </c>
-      <c r="I33" s="20">
-        <f t="shared" ref="I33:I37" si="11">C33-C32</f>
+      <c r="I36" s="20">
+        <f t="shared" ref="I36:I40" si="11">C36-C35</f>
         <v>55</v>
       </c>
-      <c r="J33" s="20">
-        <f t="shared" ref="J33:J37" si="12">(C33-C32)/(H33-H32)</f>
+      <c r="J36" s="20">
+        <f t="shared" ref="J36:J40" si="12">(C36-C35)/(H36-H35)</f>
         <v>109.15015504126526</v>
       </c>
-      <c r="K33" s="20">
-        <f t="shared" ref="K33:K37" si="13">(E33-E32)/(H33-H32)</f>
+      <c r="K36" s="20">
+        <f t="shared" ref="K36:K40" si="13">(E36-E35)/(H36-H35)</f>
         <v>1.8456298943341218</v>
       </c>
     </row>
-    <row r="34" spans="2:11">
-      <c r="B34" s="21"/>
-      <c r="C34" s="7">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="21"/>
+      <c r="C37" s="7">
         <v>1390</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D37" s="6">
         <v>700</v>
       </c>
-      <c r="E34" s="10">
+      <c r="E37" s="10">
         <v>2.4700000000000002</v>
       </c>
-      <c r="F34" s="6">
-        <f t="shared" ref="F34:F40" si="14">$D$16-D34</f>
+      <c r="F37" s="6">
+        <f t="shared" ref="F37:F43" si="14">$D$16-D37</f>
         <v>300</v>
       </c>
-      <c r="G34" s="6">
-        <f t="shared" ref="G34:G40" si="15">F34*(1-$G$12)/$G$12</f>
+      <c r="G37" s="6">
+        <f t="shared" ref="G37:G43" si="15">F37*(1-$G$12)/$G$12</f>
         <v>154.09572124826232</v>
       </c>
-      <c r="H34" s="11">
+      <c r="H37" s="11">
         <f t="shared" si="10"/>
         <v>1.5116790254454533</v>
       </c>
-      <c r="I34" s="20">
+      <c r="I37" s="20">
         <f t="shared" si="11"/>
         <v>55</v>
       </c>
-      <c r="J34" s="20">
+      <c r="J37" s="20">
         <f t="shared" si="12"/>
         <v>109.15015504126525</v>
       </c>
-      <c r="K34" s="20">
+      <c r="K37" s="20">
         <f t="shared" si="13"/>
         <v>1.8654753770688972</v>
       </c>
     </row>
-    <row r="35" spans="2:11">
-      <c r="B35" s="21"/>
-      <c r="C35" s="7">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="21"/>
+      <c r="C38" s="7">
         <v>1440</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D38" s="6">
         <v>600</v>
       </c>
-      <c r="E35" s="10">
+      <c r="E38" s="10">
         <v>3.5</v>
       </c>
-      <c r="F35" s="6">
+      <c r="F38" s="6">
         <f t="shared" si="14"/>
         <v>400</v>
       </c>
-      <c r="G35" s="6">
+      <c r="G38" s="6">
         <f t="shared" si="15"/>
         <v>205.46096166434972</v>
       </c>
-      <c r="H35" s="11">
+      <c r="H38" s="11">
         <f t="shared" si="10"/>
         <v>2.0155720339272709</v>
       </c>
-      <c r="I35" s="20">
+      <c r="I38" s="20">
         <f t="shared" si="11"/>
         <v>50</v>
       </c>
-      <c r="J35" s="20">
+      <c r="J38" s="20">
         <f t="shared" si="12"/>
         <v>99.227413673877535</v>
       </c>
-      <c r="K35" s="20">
+      <c r="K38" s="20">
         <f t="shared" si="13"/>
         <v>2.0440847216818767</v>
       </c>
     </row>
-    <row r="36" spans="2:11">
-      <c r="B36" s="21"/>
-      <c r="C36" s="7">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="21"/>
+      <c r="C39" s="7">
         <v>1495</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D39" s="6">
         <v>500</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E39" s="10">
         <v>4.3</v>
       </c>
-      <c r="F36" s="6">
+      <c r="F39" s="6">
         <f t="shared" si="14"/>
         <v>500</v>
       </c>
-      <c r="G36" s="6">
+      <c r="G39" s="6">
         <f t="shared" si="15"/>
         <v>256.82620208043721</v>
       </c>
-      <c r="H36" s="11">
+      <c r="H39" s="11">
         <f t="shared" si="10"/>
         <v>2.519465042409089</v>
       </c>
-      <c r="I36" s="20">
+      <c r="I39" s="20">
         <f t="shared" si="11"/>
         <v>55</v>
       </c>
-      <c r="J36" s="20">
+      <c r="J39" s="20">
         <f t="shared" si="12"/>
         <v>109.15015504126519</v>
       </c>
-      <c r="K36" s="20">
+      <c r="K39" s="20">
         <f t="shared" si="13"/>
         <v>1.5876386187820388</v>
       </c>
     </row>
-    <row r="37" spans="2:11">
-      <c r="B37" s="21"/>
-      <c r="C37" s="7">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="21"/>
+      <c r="C40" s="7">
         <v>1560</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D40" s="6">
         <v>400</v>
       </c>
-      <c r="E37" s="10">
+      <c r="E40" s="10">
         <v>5.47</v>
       </c>
-      <c r="F37" s="6">
+      <c r="F40" s="6">
         <f t="shared" si="14"/>
         <v>600</v>
       </c>
-      <c r="G37" s="6">
+      <c r="G40" s="6">
         <f t="shared" si="15"/>
         <v>308.19144249652464</v>
       </c>
-      <c r="H37" s="11">
+      <c r="H40" s="11">
         <f t="shared" si="10"/>
         <v>3.0233580508909066</v>
       </c>
-      <c r="I37" s="20">
+      <c r="I40" s="20">
         <f t="shared" si="11"/>
         <v>65</v>
       </c>
-      <c r="J37" s="20">
+      <c r="J40" s="20">
         <f t="shared" si="12"/>
         <v>128.99563777604081</v>
       </c>
-      <c r="K37" s="20">
+      <c r="K40" s="20">
         <f t="shared" si="13"/>
         <v>2.3219214799687342</v>
       </c>
     </row>
-    <row r="38" spans="2:11">
-      <c r="B38" s="21"/>
-      <c r="C38" s="7">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="21"/>
+      <c r="C41" s="7">
         <v>1640</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D41" s="6">
         <v>300</v>
       </c>
-      <c r="E38" s="10">
+      <c r="E41" s="10">
         <v>6.8</v>
       </c>
-      <c r="F38" s="6">
+      <c r="F41" s="6">
         <f t="shared" si="14"/>
         <v>700</v>
       </c>
-      <c r="G38" s="6">
+      <c r="G41" s="6">
         <f t="shared" si="15"/>
         <v>359.55668291261208</v>
       </c>
-      <c r="H38" s="11">
+      <c r="H41" s="11">
         <f t="shared" si="10"/>
         <v>3.5272510593727247</v>
       </c>
-      <c r="I38" s="20">
-        <f t="shared" ref="I38" si="16">C38-C37</f>
+      <c r="I41" s="20">
+        <f t="shared" ref="I41" si="16">C41-C40</f>
         <v>80</v>
       </c>
-      <c r="J38" s="20">
-        <f t="shared" ref="J38" si="17">(C38-C37)/(H38-H37)</f>
+      <c r="J41" s="20">
+        <f t="shared" ref="J41" si="17">(C41-C40)/(H41-H40)</f>
         <v>158.76386187820393</v>
       </c>
-      <c r="K38" s="20">
-        <f t="shared" ref="K38" si="18">(E38-E37)/(H38-H37)</f>
+      <c r="K41" s="20">
+        <f t="shared" ref="K41" si="18">(E41-E40)/(H41-H40)</f>
         <v>2.6394492037251402</v>
       </c>
     </row>
-    <row r="39" spans="2:11">
-      <c r="B39" s="21"/>
-      <c r="C39" s="7">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="21"/>
+      <c r="C42" s="7">
         <v>1690</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D42" s="6">
         <v>200</v>
       </c>
-      <c r="E39" s="10">
+      <c r="E42" s="10">
         <v>8.1</v>
       </c>
-      <c r="F39" s="6">
+      <c r="F42" s="6">
         <f t="shared" si="14"/>
         <v>800</v>
       </c>
-      <c r="G39" s="6">
+      <c r="G42" s="6">
         <f t="shared" si="15"/>
         <v>410.92192332869945</v>
       </c>
-      <c r="H39" s="11">
+      <c r="H42" s="11">
         <f t="shared" si="10"/>
         <v>4.0311440678545418</v>
       </c>
-      <c r="I39" s="20">
-        <f t="shared" ref="I39:I40" si="19">C39-C38</f>
+      <c r="I42" s="20">
+        <f t="shared" ref="I42:I43" si="19">C42-C41</f>
         <v>50</v>
       </c>
-      <c r="J39" s="20">
-        <f t="shared" ref="J39:J40" si="20">(C39-C38)/(H39-H38)</f>
+      <c r="J42" s="20">
+        <f t="shared" ref="J42:J43" si="20">(C42-C41)/(H42-H41)</f>
         <v>99.227413673877621</v>
       </c>
-      <c r="K39" s="20">
-        <f t="shared" ref="K39:K40" si="21">(E39-E38)/(H39-H38)</f>
+      <c r="K42" s="20">
+        <f t="shared" ref="K42:K43" si="21">(E42-E41)/(H42-H41)</f>
         <v>2.5799127555208181</v>
       </c>
     </row>
-    <row r="40" spans="2:11">
-      <c r="B40" s="21"/>
-      <c r="C40" s="7">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="21"/>
+      <c r="C43" s="7">
         <v>1740</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D43" s="6">
         <v>100</v>
       </c>
-      <c r="E40" s="10">
+      <c r="E43" s="10">
         <v>10</v>
       </c>
-      <c r="F40" s="6">
+      <c r="F43" s="6">
         <f t="shared" si="14"/>
         <v>900</v>
       </c>
-      <c r="G40" s="6">
+      <c r="G43" s="6">
         <f t="shared" si="15"/>
         <v>462.28716374478694</v>
       </c>
-      <c r="H40" s="11">
+      <c r="H43" s="11">
         <f t="shared" si="10"/>
         <v>4.5350370763363594</v>
       </c>
-      <c r="I40" s="20">
+      <c r="I43" s="20">
         <f t="shared" si="19"/>
         <v>50</v>
       </c>
-      <c r="J40" s="20">
+      <c r="J43" s="20">
         <f t="shared" si="20"/>
         <v>99.227413673877535</v>
       </c>
-      <c r="K40" s="20">
+      <c r="K43" s="20">
         <f t="shared" si="21"/>
         <v>3.7706417196073474</v>
       </c>
     </row>
-    <row r="41" spans="2:11">
-      <c r="B41" s="1"/>
-    </row>
-    <row r="42" spans="2:11" ht="15" customHeight="1">
-      <c r="B42" s="21" t="s">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C45">
+        <f>SLOPE(C34:C43,H34:H43)</f>
+        <v>114.86324855582188</v>
+      </c>
+      <c r="E45" s="24">
+        <f>SLOPE(E34:E43,C34:C43)</f>
+        <v>1.8715316615551144E-2</v>
+      </c>
+      <c r="H45" s="25">
+        <f>SLOPE(H34:H43,C34:C43)</f>
+        <v>8.6815410986854774E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C46">
+        <f>INTERCEPT(C34:C43,H34:H43)</f>
+        <v>1219.5454545454545</v>
+      </c>
+      <c r="E46" s="22">
+        <f>INTERCEPT(E34:E43,C34:C43)</f>
+        <v>-23.421668591015695</v>
+      </c>
+      <c r="H46" s="23">
+        <f>INTERCEPT(H34:H43,C34:C43)</f>
+        <v>-10.581162287886325</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="G48" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="H48" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I42" s="18" t="s">
+      <c r="I48" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="J42" s="18" t="s">
+      <c r="J48" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="K42" s="18" t="s">
+      <c r="K48" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="2:11">
-      <c r="B43" s="21"/>
-      <c r="C43" s="7">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B49" s="21"/>
+      <c r="C49" s="7">
         <v>1230</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D49" s="6">
         <v>1000</v>
       </c>
-      <c r="E43" s="10">
+      <c r="E49" s="10">
         <v>0</v>
       </c>
-      <c r="F43" s="6">
-        <f>$D$16-D43</f>
+      <c r="F49" s="6">
+        <f>$D$16-D49</f>
         <v>0</v>
       </c>
-      <c r="G43" s="6">
-        <f>F43*(1-$G$12)/$G$12</f>
+      <c r="G49" s="6">
+        <f>F49*(1-$G$12)/$G$12</f>
         <v>0</v>
       </c>
-      <c r="H43" s="11">
-        <f>G43*$G$5/1000</f>
+      <c r="H49" s="11">
+        <f>G49*$G$5/1000</f>
         <v>0</v>
       </c>
-      <c r="I43" s="19" t="s">
+      <c r="I49" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="J43" s="19" t="s">
+      <c r="J49" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="K43" s="19" t="s">
+      <c r="K49" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="2:11">
-      <c r="B44" s="21"/>
-      <c r="C44" s="7">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B50" s="21"/>
+      <c r="C50" s="7">
         <v>1275</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D50" s="6">
         <v>900</v>
       </c>
-      <c r="E44" s="10">
+      <c r="E50" s="10">
         <v>0.53</v>
       </c>
-      <c r="F44" s="6">
-        <f t="shared" ref="F44:F45" si="22">$D$16-D44</f>
+      <c r="F50" s="6">
+        <f t="shared" ref="F50:F51" si="22">$D$16-D50</f>
         <v>100</v>
       </c>
-      <c r="G44" s="6">
-        <f t="shared" ref="G44:G45" si="23">F44*(1-$G$12)/$G$12</f>
+      <c r="G50" s="6">
+        <f t="shared" ref="G50:G51" si="23">F50*(1-$G$12)/$G$12</f>
         <v>51.365240416087431</v>
       </c>
-      <c r="H44" s="11">
-        <f t="shared" ref="H44:H53" si="24">G44*$G$5/1000</f>
+      <c r="H50" s="11">
+        <f t="shared" ref="H50:H59" si="24">G50*$G$5/1000</f>
         <v>0.50389300848181773</v>
       </c>
-      <c r="I44" s="20">
-        <f>C44-C43</f>
+      <c r="I50" s="20">
+        <f>C50-C49</f>
         <v>45</v>
       </c>
-      <c r="J44" s="20">
-        <f>(C44-C43)/(H44-H43)</f>
+      <c r="J50" s="20">
+        <f>(C50-C49)/(H50-H49)</f>
         <v>89.304672306489763</v>
       </c>
-      <c r="K44" s="20">
-        <f>(E44-E43)/(H44-H43)</f>
+      <c r="K50" s="20">
+        <f>(E50-E49)/(H50-H49)</f>
         <v>1.0518105849431016</v>
       </c>
     </row>
-    <row r="45" spans="2:11">
-      <c r="B45" s="21"/>
-      <c r="C45" s="7">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B51" s="21"/>
+      <c r="C51" s="7">
         <v>1325</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D51" s="6">
         <v>800</v>
       </c>
-      <c r="E45" s="10">
+      <c r="E51" s="10">
         <v>1.4</v>
       </c>
-      <c r="F45" s="6">
+      <c r="F51" s="6">
         <f t="shared" si="22"/>
         <v>200</v>
       </c>
-      <c r="G45" s="6">
+      <c r="G51" s="6">
         <f t="shared" si="23"/>
         <v>102.73048083217486</v>
       </c>
-      <c r="H45" s="11">
+      <c r="H51" s="11">
         <f t="shared" si="24"/>
         <v>1.0077860169636355</v>
       </c>
-      <c r="I45" s="20">
-        <f t="shared" ref="I45:I52" si="25">C45-C44</f>
+      <c r="I51" s="20">
+        <f t="shared" ref="I51:I58" si="25">C51-C50</f>
         <v>50</v>
       </c>
-      <c r="J45" s="20">
-        <f t="shared" ref="J45:J52" si="26">(C45-C44)/(H45-H44)</f>
+      <c r="J51" s="20">
+        <f t="shared" ref="J51:J58" si="26">(C51-C50)/(H51-H50)</f>
         <v>99.227413673877521</v>
       </c>
-      <c r="K45" s="20">
-        <f t="shared" ref="K45:K52" si="27">(E45-E44)/(H45-H44)</f>
+      <c r="K51" s="20">
+        <f t="shared" ref="K51:K58" si="27">(E51-E50)/(H51-H50)</f>
         <v>1.7265569979254685</v>
       </c>
     </row>
-    <row r="46" spans="2:11">
-      <c r="B46" s="21"/>
-      <c r="C46" s="7">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B52" s="21"/>
+      <c r="C52" s="7">
         <v>1375</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D52" s="6">
         <v>700</v>
       </c>
-      <c r="E46" s="10">
+      <c r="E52" s="10">
         <v>2.33</v>
       </c>
-      <c r="F46" s="6">
-        <f>$D$16-D46</f>
+      <c r="F52" s="6">
+        <f>$D$16-D52</f>
         <v>300</v>
       </c>
-      <c r="G46" s="6">
-        <f>F46*(1-$G$12)/$G$12</f>
+      <c r="G52" s="6">
+        <f>F52*(1-$G$12)/$G$12</f>
         <v>154.09572124826232</v>
       </c>
-      <c r="H46" s="11">
+      <c r="H52" s="11">
         <f t="shared" si="24"/>
         <v>1.5116790254454533</v>
       </c>
-      <c r="I46" s="20">
+      <c r="I52" s="20">
         <f t="shared" si="25"/>
         <v>50</v>
       </c>
-      <c r="J46" s="20">
+      <c r="J52" s="20">
         <f t="shared" si="26"/>
         <v>99.227413673877493</v>
       </c>
-      <c r="K46" s="20">
+      <c r="K52" s="20">
         <f t="shared" si="27"/>
         <v>1.8456298943341218</v>
       </c>
     </row>
-    <row r="47" spans="2:11">
-      <c r="B47" s="21"/>
-      <c r="C47" s="7">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B53" s="21"/>
+      <c r="C53" s="7">
         <v>1420</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D53" s="6">
         <v>600</v>
       </c>
-      <c r="E47" s="10">
+      <c r="E53" s="10">
         <v>3.2</v>
       </c>
-      <c r="F47" s="6">
-        <f>$D$16-D47</f>
+      <c r="F53" s="6">
+        <f>$D$16-D53</f>
         <v>400</v>
       </c>
-      <c r="G47" s="6">
-        <f>F47*(1-$G$12)/$G$12</f>
+      <c r="G53" s="6">
+        <f>F53*(1-$G$12)/$G$12</f>
         <v>205.46096166434972</v>
       </c>
-      <c r="H47" s="11">
+      <c r="H53" s="11">
         <f t="shared" si="24"/>
         <v>2.0155720339272709</v>
       </c>
-      <c r="I47" s="20">
+      <c r="I53" s="20">
         <f t="shared" si="25"/>
         <v>45</v>
       </c>
-      <c r="J47" s="20">
+      <c r="J53" s="20">
         <f t="shared" si="26"/>
         <v>89.304672306489792</v>
       </c>
-      <c r="K47" s="20">
+      <c r="K53" s="20">
         <f t="shared" si="27"/>
         <v>1.7265569979254694</v>
       </c>
     </row>
-    <row r="48" spans="2:11">
-      <c r="B48" s="21"/>
-      <c r="C48" s="7">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B54" s="21"/>
+      <c r="C54" s="7">
         <v>1450</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D54" s="6">
         <v>500</v>
       </c>
-      <c r="E48" s="10">
+      <c r="E54" s="10">
         <v>4.34</v>
       </c>
-      <c r="F48" s="6">
-        <f>$D$16-D48</f>
+      <c r="F54" s="6">
+        <f>$D$16-D54</f>
         <v>500</v>
       </c>
-      <c r="G48" s="6">
-        <f>F48*(1-$G$12)/$G$12</f>
+      <c r="G54" s="6">
+        <f>F54*(1-$G$12)/$G$12</f>
         <v>256.82620208043721</v>
       </c>
-      <c r="H48" s="11">
+      <c r="H54" s="11">
         <f t="shared" si="24"/>
         <v>2.519465042409089</v>
       </c>
-      <c r="I48" s="20">
+      <c r="I54" s="20">
         <f t="shared" si="25"/>
         <v>30</v>
       </c>
-      <c r="J48" s="20">
+      <c r="J54" s="20">
         <f t="shared" si="26"/>
         <v>59.536448204326469</v>
       </c>
-      <c r="K48" s="20">
+      <c r="K54" s="20">
         <f t="shared" si="27"/>
         <v>2.2623850317644054</v>
       </c>
     </row>
-    <row r="49" spans="2:11">
-      <c r="B49" s="21"/>
-      <c r="C49" s="7">
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B55" s="21"/>
+      <c r="C55" s="7">
         <v>1505</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D55" s="6">
         <v>400</v>
       </c>
-      <c r="E49" s="10">
+      <c r="E55" s="10">
         <v>5.54</v>
       </c>
-      <c r="F49" s="6">
-        <f t="shared" ref="F49:F53" si="28">$D$16-D49</f>
+      <c r="F55" s="6">
+        <f t="shared" ref="F55:F59" si="28">$D$16-D55</f>
         <v>600</v>
       </c>
-      <c r="G49" s="6">
-        <f t="shared" ref="G49:G53" si="29">F49*(1-$G$12)/$G$12</f>
+      <c r="G55" s="6">
+        <f t="shared" ref="G55:G59" si="29">F55*(1-$G$12)/$G$12</f>
         <v>308.19144249652464</v>
       </c>
-      <c r="H49" s="11">
+      <c r="H55" s="11">
         <f t="shared" si="24"/>
         <v>3.0233580508909066</v>
       </c>
-      <c r="I49" s="20">
+      <c r="I55" s="20">
         <f t="shared" si="25"/>
         <v>55</v>
       </c>
-      <c r="J49" s="20">
+      <c r="J55" s="20">
         <f t="shared" si="26"/>
         <v>109.15015504126529</v>
       </c>
-      <c r="K49" s="20">
+      <c r="K55" s="20">
         <f t="shared" si="27"/>
         <v>2.3814579281730612</v>
       </c>
     </row>
-    <row r="50" spans="2:11">
-      <c r="B50" s="21"/>
-      <c r="C50" s="7">
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B56" s="21"/>
+      <c r="C56" s="7">
         <v>1560</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D56" s="6">
         <v>300</v>
       </c>
-      <c r="E50" s="10">
+      <c r="E56" s="10">
         <v>6.2</v>
       </c>
-      <c r="F50" s="6">
+      <c r="F56" s="6">
         <f t="shared" si="28"/>
         <v>700</v>
       </c>
-      <c r="G50" s="6">
+      <c r="G56" s="6">
         <f t="shared" si="29"/>
         <v>359.55668291261208</v>
       </c>
-      <c r="H50" s="11">
+      <c r="H56" s="11">
         <f t="shared" si="24"/>
         <v>3.5272510593727247</v>
       </c>
-      <c r="I50" s="20">
+      <c r="I56" s="20">
         <f t="shared" si="25"/>
         <v>55</v>
       </c>
-      <c r="J50" s="20">
+      <c r="J56" s="20">
         <f t="shared" si="26"/>
         <v>109.15015504126519</v>
       </c>
-      <c r="K50" s="20">
+      <c r="K56" s="20">
         <f t="shared" si="27"/>
         <v>1.3098018604951827</v>
       </c>
     </row>
-    <row r="51" spans="2:11">
-      <c r="B51" s="21"/>
-      <c r="C51" s="7">
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B57" s="21"/>
+      <c r="C57" s="7">
         <v>1620</v>
       </c>
-      <c r="D51" s="6">
+      <c r="D57" s="6">
         <v>200</v>
       </c>
-      <c r="E51" s="10">
+      <c r="E57" s="10">
         <v>7.6</v>
       </c>
-      <c r="F51" s="6">
+      <c r="F57" s="6">
         <f t="shared" si="28"/>
         <v>800</v>
       </c>
-      <c r="G51" s="6">
+      <c r="G57" s="6">
         <f t="shared" si="29"/>
         <v>410.92192332869945</v>
       </c>
-      <c r="H51" s="11">
+      <c r="H57" s="11">
         <f t="shared" si="24"/>
         <v>4.0311440678545418</v>
       </c>
-      <c r="I51" s="20">
+      <c r="I57" s="20">
         <f t="shared" si="25"/>
         <v>60</v>
       </c>
-      <c r="J51" s="20">
+      <c r="J57" s="20">
         <f t="shared" si="26"/>
         <v>119.07289640865315</v>
       </c>
-      <c r="K51" s="20">
+      <c r="K57" s="20">
         <f t="shared" si="27"/>
         <v>2.7783675828685723</v>
       </c>
     </row>
-    <row r="52" spans="2:11">
-      <c r="B52" s="21"/>
-      <c r="C52" s="7">
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B58" s="21"/>
+      <c r="C58" s="7">
         <v>1650</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D58" s="6">
         <v>100</v>
       </c>
-      <c r="E52" s="10">
+      <c r="E58" s="10">
         <v>8.1999999999999993</v>
       </c>
-      <c r="F52" s="6">
+      <c r="F58" s="6">
         <f t="shared" si="28"/>
         <v>900</v>
       </c>
-      <c r="G52" s="6">
+      <c r="G58" s="6">
         <f t="shared" si="29"/>
         <v>462.28716374478694</v>
       </c>
-      <c r="H52" s="11">
+      <c r="H58" s="11">
         <f t="shared" si="24"/>
         <v>4.5350370763363594</v>
       </c>
-      <c r="I52" s="20">
+      <c r="I58" s="20">
         <f t="shared" si="25"/>
         <v>30</v>
       </c>
-      <c r="J52" s="20">
+      <c r="J58" s="20">
         <f t="shared" si="26"/>
         <v>59.536448204326526</v>
       </c>
-      <c r="K52" s="20">
+      <c r="K58" s="20">
         <f t="shared" si="27"/>
         <v>1.1907289640865297</v>
       </c>
     </row>
-    <row r="53" spans="2:11">
-      <c r="B53" s="21"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="6">
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B59" s="21"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="6">
         <v>0</v>
       </c>
-      <c r="E53" s="10"/>
-      <c r="F53" s="6">
+      <c r="E59" s="10"/>
+      <c r="F59" s="6">
         <f t="shared" si="28"/>
         <v>1000</v>
       </c>
-      <c r="G53" s="6">
+      <c r="G59" s="6">
         <f t="shared" si="29"/>
         <v>513.65240416087443</v>
       </c>
-      <c r="H53" s="11">
+      <c r="H59" s="11">
         <f t="shared" si="24"/>
         <v>5.0389300848181779</v>
       </c>
-      <c r="I53" s="20"/>
-      <c r="J53" s="20"/>
-      <c r="K53" s="20"/>
-    </row>
-    <row r="55" spans="2:11">
-      <c r="D55" s="1" t="s">
+      <c r="I59" s="20"/>
+      <c r="J59" s="20"/>
+      <c r="K59" s="20"/>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61">
+        <f>SLOPE(C49:C59,H49:H59)</f>
+        <v>93.694733638727968</v>
+      </c>
+      <c r="E61" s="24">
+        <f>SLOPE(E49:E59,C49:C59)</f>
+        <v>2.0251965941753887E-2</v>
+      </c>
+      <c r="H61" s="25">
+        <f>SLOPE(H49:H59,C49:C59)</f>
+        <v>1.0644087358515537E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C62">
+        <f>INTERCEPT(C49:C59,H49:H59)</f>
+        <v>1228.5454545454545</v>
+      </c>
+      <c r="E62" s="22">
+        <f>INTERCEPT(E49:E59,C49:C59)</f>
+        <v>-25.249082922067348</v>
+      </c>
+      <c r="H62" s="23">
+        <f>INTERCEPT(H49:H59,C49:C59)</f>
+        <v>-13.070611345452708</v>
+      </c>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D64" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="E64" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F55" s="12">
+      <c r="F64" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:11">
-      <c r="C56" s="14" t="s">
+    <row r="65" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C65" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D56" s="7" t="e">
-        <f t="array" ref="D56:F56">LINEST(E19:E25,H19:H25^{1,2})</f>
+      <c r="D65" s="7" t="e">
+        <f t="array" ref="D65:F65">LINEST(E19:E25,H19:H25^{1,2})</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E56" s="7" t="e">
+      <c r="E65" s="7" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="F56" s="7" t="e">
+      <c r="F65" s="7" t="e">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="57" spans="2:11">
-      <c r="C57" s="13" t="s">
+    <row r="66" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C66" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D57" s="7" t="e">
-        <f t="array" ref="D57:F57">LINEST(C19:C25,H19:H25^{1,2})</f>
+      <c r="D66" s="7" t="e">
+        <f t="array" ref="D66:F66">LINEST(C19:C25,H19:H25^{1,2})</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E57" s="7" t="e">
+      <c r="E66" s="7" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="F57" s="7" t="e">
+      <c r="F66" s="7" t="e">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="58" spans="2:11">
-      <c r="C58" s="1" t="s">
+    <row r="67" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C67" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D58" s="11">
+      <c r="D67" s="11">
         <v>2.9554404442782194</v>
       </c>
-      <c r="E58" s="6">
-        <f>1000*D58/G5</f>
+      <c r="E67" s="6">
+        <f>1000*D67/G5</f>
         <v>301.26813907015486</v>
       </c>
-      <c r="F58" s="6">
-        <f>E58*$G$12/(1-$G$12)</f>
+      <c r="F67" s="6">
+        <f>E67*$G$12/(1-$G$12)</f>
         <v>586.52142310580632</v>
       </c>
     </row>
-    <row r="59" spans="2:11">
-      <c r="C59" s="1" t="s">
+    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C68" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D59" s="15" t="e">
-        <f>D57*D58*D58+E57*D58+F57</f>
+      <c r="D68" s="15" t="e">
+        <f>D66*D67*D67+E66*D67+F66</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E59" s="6"/>
-      <c r="F59" s="7"/>
-    </row>
-    <row r="60" spans="2:11">
-      <c r="C60" s="1" t="s">
+      <c r="E68" s="6"/>
+      <c r="F68" s="7"/>
+    </row>
+    <row r="69" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C69" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D60" s="10">
+      <c r="D69" s="10">
         <v>11</v>
       </c>
-      <c r="E60" s="7"/>
-      <c r="F60" s="7"/>
-    </row>
-    <row r="61" spans="2:11">
-      <c r="C61" s="1" t="s">
+      <c r="E69" s="7"/>
+      <c r="F69" s="7"/>
+    </row>
+    <row r="70" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C70" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D61" s="7" t="e">
-        <f>D56*D58*D58+E56*D58+F56-D60</f>
+      <c r="D70" s="7" t="e">
+        <f>D65*D67*D67+E65*D67+F65-D69</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E61" s="7"/>
-      <c r="F61" s="7"/>
-    </row>
-    <row r="63" spans="2:11">
-      <c r="C63" s="1" t="s">
+      <c r="E70" s="7"/>
+      <c r="F70" s="7"/>
+    </row>
+    <row r="72" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C72" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D63" s="11">
-        <f>3*D58</f>
+      <c r="D72" s="11">
+        <f>3*D67</f>
         <v>8.8663213328346586</v>
       </c>
     </row>
-    <row r="64" spans="2:11">
-      <c r="C64" s="1" t="s">
+    <row r="73" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C73" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D64" s="6">
+      <c r="D73" s="6">
         <v>550</v>
       </c>
     </row>
-    <row r="65" spans="3:4">
-      <c r="C65" s="1" t="s">
+    <row r="74" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C74" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D65" s="4">
-        <f>D63/(D64/1000)</f>
+      <c r="D74" s="4">
+        <f>D72/(D73/1000)</f>
         <v>16.120584241517559</v>
       </c>
     </row>
-    <row r="66" spans="3:4">
-      <c r="C66" s="1" t="s">
+    <row r="75" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C75" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D66" s="4">
-        <f>D65-G5</f>
+      <c r="D75" s="4">
+        <f>D74-G5</f>
         <v>6.3105842415175584</v>
       </c>
     </row>
-    <row r="67" spans="3:4">
-      <c r="C67" s="1" t="s">
+    <row r="76" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C76" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D67" s="16">
-        <f>D66*10*3.6</f>
+      <c r="D76" s="16">
+        <f>D75*10*3.6</f>
         <v>227.18103269463211</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B30:B40"/>
+    <mergeCell ref="B33:B43"/>
     <mergeCell ref="B18:B28"/>
-    <mergeCell ref="B42:B53"/>
+    <mergeCell ref="B48:B59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5294,16 +5562,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:10">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>56</v>
       </c>
@@ -5311,7 +5579,7 @@
         <v>2.65</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>41</v>
       </c>
@@ -5319,7 +5587,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>39</v>
       </c>
@@ -5345,7 +5613,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>37</v>
       </c>
@@ -5379,7 +5647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>38</v>
       </c>
@@ -5415,7 +5683,7 @@
         <v>18.654461889485574</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>42</v>
       </c>
@@ -5451,7 +5719,7 @@
         <v>27.272952676572356</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>43</v>
       </c>
@@ -5487,7 +5755,7 @@
         <v>31.862747612613184</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>44</v>
       </c>
@@ -5523,7 +5791,7 @@
         <v>34.462018318825038</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>45</v>
       </c>
@@ -5559,7 +5827,7 @@
         <v>35.950364522126321</v>
       </c>
     </row>
-    <row r="13" spans="2:10">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>46</v>
       </c>
@@ -5595,7 +5863,7 @@
         <v>36.767781993202043</v>
       </c>
     </row>
-    <row r="14" spans="2:10">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>47</v>
       </c>
@@ -5631,7 +5899,7 @@
         <v>37.157571812040167</v>
       </c>
     </row>
-    <row r="15" spans="2:10">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>48</v>
       </c>
@@ -5667,7 +5935,7 @@
         <v>37.264361954949486</v>
       </c>
     </row>
-    <row r="16" spans="2:10">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>49</v>
       </c>
@@ -5703,7 +5971,7 @@
         <v>37.178926947153002</v>
       </c>
     </row>
-    <row r="17" spans="2:10">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>50</v>
       </c>
@@ -5739,7 +6007,7 @@
         <v>36.960684501829995</v>
       </c>
     </row>
-    <row r="18" spans="2:10">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>51</v>
       </c>
@@ -5775,7 +6043,7 @@
         <v>36.649836004687224</v>
       </c>
     </row>
-    <row r="19" spans="2:10">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>52</v>
       </c>
@@ -5811,7 +6079,7 @@
         <v>36.274309264908197</v>
       </c>
     </row>
-    <row r="20" spans="2:10">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>53</v>
       </c>
@@ -5847,7 +6115,7 @@
         <v>35.853921683595352</v>
       </c>
     </row>
-    <row r="21" spans="2:10">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>54</v>
       </c>
@@ -5883,7 +6151,7 @@
         <v>35.402977202193746</v>
       </c>
     </row>
-    <row r="22" spans="2:10">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>60</v>
       </c>
@@ -5919,7 +6187,7 @@
         <v>34.931941166266107</v>
       </c>
     </row>
-    <row r="23" spans="2:10">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>61</v>
       </c>
@@ -5955,7 +6223,7 @@
         <v>34.448551696900424</v>
       </c>
     </row>
-    <row r="24" spans="2:10">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>62</v>
       </c>
@@ -5991,7 +6259,7 @@
         <v>33.958575475877865</v>
       </c>
     </row>
-    <row r="25" spans="2:10">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>63</v>
       </c>
@@ -6027,7 +6295,7 @@
         <v>33.466332795437836</v>
       </c>
     </row>
-    <row r="26" spans="2:10">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>64</v>
       </c>
@@ -6063,7 +6331,7 @@
         <v>32.975069183398517</v>
       </c>
     </row>
-    <row r="27" spans="2:10">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>65</v>
       </c>
@@ -6099,7 +6367,7 @@
         <v>32.487222787312376</v>
       </c>
     </row>
-    <row r="28" spans="2:10">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>66</v>
       </c>
@@ -6135,7 +6403,7 @@
         <v>32.004619566108737</v>
       </c>
     </row>
-    <row r="29" spans="2:10">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>67</v>
       </c>
@@ -6171,7 +6439,7 @@
         <v>31.528617623502459</v>
       </c>
     </row>
-    <row r="30" spans="2:10">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>68</v>
       </c>
@@ -6207,7 +6475,7 @@
         <v>31.060215160191568</v>
       </c>
     </row>
-    <row r="31" spans="2:10">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>69</v>
       </c>
@@ -6243,7 +6511,7 @@
         <v>30.600132040015254</v>
       </c>
     </row>
-    <row r="32" spans="2:10">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>70</v>
       </c>
@@ -6279,7 +6547,7 @@
         <v>30.148871979776708</v>
       </c>
     </row>
-    <row r="33" spans="2:10">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>71</v>
       </c>
@@ -6315,7 +6583,7 @@
         <v>29.706770349127993</v>
       </c>
     </row>
-    <row r="34" spans="2:10">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>72</v>
       </c>
@@ -6351,7 +6619,7 @@
         <v>29.274031173921884</v>
       </c>
     </row>
-    <row r="35" spans="2:10">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>73</v>
       </c>
@@ -6387,7 +6655,7 @@
         <v>28.850755963478811</v>
       </c>
     </row>
-    <row r="36" spans="2:10">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>74</v>
       </c>
@@ -6423,7 +6691,7 @@
         <v>28.436966293588206</v>
       </c>
     </row>
-    <row r="37" spans="2:10">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>75</v>
       </c>
@@ -6459,7 +6727,7 @@
         <v>28.032621583698859</v>
       </c>
     </row>
-    <row r="38" spans="2:10">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>76</v>
       </c>
@@ -6495,7 +6763,7 @@
         <v>27.637633149284962</v>
       </c>
     </row>
-    <row r="39" spans="2:10">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>77</v>
       </c>
@@ -6531,7 +6799,7 @@
         <v>27.251875348663212</v>
       </c>
     </row>
-    <row r="40" spans="2:10">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>78</v>
       </c>
@@ -6567,7 +6835,7 @@
         <v>26.875194450070506</v>
       </c>
     </row>
-    <row r="41" spans="2:10">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>79</v>
       </c>
@@ -6603,7 +6871,7 @@
         <v>26.507415700509842</v>
       </c>
     </row>
-    <row r="42" spans="2:10">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>80</v>
       </c>
@@ -6639,7 +6907,7 @@
         <v>26.148348969337157</v>
       </c>
     </row>
-    <row r="43" spans="2:10">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>81</v>
       </c>
@@ -6675,7 +6943,7 @@
         <v>25.797793257292437</v>
       </c>
     </row>
-    <row r="44" spans="2:10">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>82</v>
       </c>
@@ -6711,7 +6979,7 @@
         <v>25.455540298864697</v>
       </c>
     </row>
-    <row r="45" spans="2:10">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>83</v>
       </c>
@@ -6747,7 +7015,7 @@
         <v>25.12137743759358</v>
       </c>
     </row>
-    <row r="46" spans="2:10">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>84</v>
       </c>
@@ -6783,7 +7051,7 @@
         <v>24.795089916556982</v>
       </c>
     </row>
-    <row r="47" spans="2:10">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>85</v>
       </c>
@@ -6819,7 +7087,7 @@
         <v>24.476462697224498</v>
       </c>
     </row>
-    <row r="48" spans="2:10">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>86</v>
       </c>
@@ -6855,7 +7123,7 @@
         <v>24.165281897109335</v>
       </c>
     </row>
-    <row r="49" spans="2:10">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>87</v>
       </c>
@@ -6891,7 +7159,7 @@
         <v>23.861335918757071</v>
       </c>
     </row>
-    <row r="50" spans="2:10">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>88</v>
       </c>
@@ -6927,7 +7195,7 @@
         <v>23.564416328465377</v>
       </c>
     </row>
-    <row r="51" spans="2:10">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>89</v>
       </c>
@@ -6963,7 +7231,7 @@
         <v>23.274318531896412</v>
       </c>
     </row>
-    <row r="52" spans="2:10">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>90</v>
       </c>
@@ -6999,7 +7267,7 @@
         <v>22.990842284786176</v>
       </c>
     </row>
-    <row r="53" spans="2:10">
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>91</v>
       </c>
@@ -7035,7 +7303,7 @@
         <v>22.713792069782041</v>
       </c>
     </row>
-    <row r="54" spans="2:10">
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>92</v>
       </c>
@@ -7071,7 +7339,7 @@
         <v>22.44297736467519</v>
       </c>
     </row>
-    <row r="55" spans="2:10">
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>93</v>
       </c>
@@ -7107,7 +7375,7 @@
         <v>22.178212822644625</v>
       </c>
     </row>
-    <row r="56" spans="2:10">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>94</v>
       </c>
@@ -7143,7 +7411,7 @@
         <v>21.919318381366896</v>
       </c>
     </row>
-    <row r="57" spans="2:10">
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>95</v>
       </c>
@@ -7179,7 +7447,7 @@
         <v>21.666119314791391</v>
       </c>
     </row>
-    <row r="58" spans="2:10">
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>96</v>
       </c>
@@ -7215,7 +7483,7 @@
         <v>21.418446238895051</v>
       </c>
     </row>
-    <row r="59" spans="2:10">
+    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>97</v>
       </c>
@@ -7251,7 +7519,7 @@
         <v>21.176135080701062</v>
       </c>
     </row>
-    <row r="60" spans="2:10">
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>98</v>
       </c>
@@ -7287,7 +7555,7 @@
         <v>20.939027018186433</v>
       </c>
     </row>
-    <row r="61" spans="2:10">
+    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>99</v>
       </c>
@@ -7323,7 +7591,7 @@
         <v>20.706968397341399</v>
       </c>
     </row>
-    <row r="62" spans="2:10">
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>100</v>
       </c>
@@ -7359,7 +7627,7 @@
         <v>20.479810631526277</v>
       </c>
     </row>
-    <row r="63" spans="2:10">
+    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>101</v>
       </c>
@@ -7395,7 +7663,7 @@
         <v>20.257410087349495</v>
       </c>
     </row>
-    <row r="64" spans="2:10">
+    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>102</v>
       </c>
@@ -7431,7 +7699,7 @@
         <v>20.039627960532616</v>
       </c>
     </row>
-    <row r="65" spans="2:10">
+    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>103</v>
       </c>
@@ -7467,7 +7735,7 @@
         <v>19.826330144600746</v>
       </c>
     </row>
-    <row r="66" spans="2:10">
+    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>104</v>
       </c>
@@ -7503,7 +7771,7 @@
         <v>19.617387094718776</v>
       </c>
     </row>
-    <row r="67" spans="2:10">
+    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>105</v>
       </c>
@@ -7539,7 +7807,7 @@
         <v>19.412673688565533</v>
       </c>
     </row>
-    <row r="68" spans="2:10">
+    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>106</v>
       </c>
@@ -7575,7 +7843,7 @@
         <v>19.212069085782154</v>
       </c>
     </row>
-    <row r="69" spans="2:10">
+    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>107</v>
       </c>
@@ -7611,7 +7879,7 @@
         <v>19.015456587237541</v>
       </c>
     </row>
-    <row r="70" spans="2:10">
+    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>108</v>
       </c>
@@ -7647,7 +7915,7 @@
         <v>18.822723495109351</v>
       </c>
     </row>
-    <row r="71" spans="2:10">
+    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>109</v>
       </c>
@@ -7683,7 +7951,7 @@
         <v>18.63376097457699</v>
       </c>
     </row>
-    <row r="72" spans="2:10">
+    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>110</v>
       </c>
@@ -7703,7 +7971,7 @@
         <v>115.13016000000002</v>
       </c>
       <c r="G72">
-        <f t="shared" ref="G72:G135" si="11">F72/3</f>
+        <f t="shared" ref="G72:G83" si="11">F72/3</f>
         <v>38.376720000000006</v>
       </c>
       <c r="H72">
@@ -7711,7 +7979,7 @@
         <v>186.73641422711427</v>
       </c>
       <c r="I72">
-        <f t="shared" ref="I72:I135" si="13">H72*3</f>
+        <f t="shared" ref="I72:I83" si="13">H72*3</f>
         <v>560.20924268134286</v>
       </c>
       <c r="J72">
@@ -7719,16 +7987,16 @@
         <v>18.448463917755699</v>
       </c>
     </row>
-    <row r="73" spans="2:10">
+    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>111</v>
       </c>
       <c r="C73">
-        <f t="shared" ref="C73:C136" si="14">$C$7+E73*$C$4</f>
+        <f t="shared" ref="C73:C83" si="14">$C$7+E73*$C$4</f>
         <v>11911</v>
       </c>
       <c r="D73">
-        <f t="shared" ref="D73:D136" si="15">$D$7+E73*$C$3</f>
+        <f t="shared" ref="D73:D83" si="15">$D$7+E73*$C$3</f>
         <v>174.9</v>
       </c>
       <c r="E73">
@@ -7755,7 +8023,7 @@
         <v>18.266730810361871</v>
       </c>
     </row>
-    <row r="74" spans="2:10">
+    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>112</v>
       </c>
@@ -7791,7 +8059,7 @@
         <v>18.088463601485067</v>
       </c>
     </row>
-    <row r="75" spans="2:10">
+    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>113</v>
       </c>
@@ -7807,7 +8075,7 @@
         <v>68</v>
       </c>
       <c r="F75">
-        <f t="shared" ref="F75:F88" si="16">C75/1000*9.81</f>
+        <f t="shared" ref="F75:F83" si="16">C75/1000*9.81</f>
         <v>120.28041</v>
       </c>
       <c r="G75">
@@ -7823,11 +8091,11 @@
         <v>603.56486521615136</v>
       </c>
       <c r="J75">
-        <f t="shared" ref="J75:J88" si="17">D75/I75*60</f>
+        <f t="shared" ref="J75:J83" si="17">D75/I75*60</f>
         <v>17.913567576747461</v>
       </c>
     </row>
-    <row r="76" spans="2:10">
+    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>114</v>
       </c>
@@ -7863,7 +8131,7 @@
         <v>17.741951235052856</v>
       </c>
     </row>
-    <row r="77" spans="2:10">
+    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>115</v>
       </c>
@@ -7899,7 +8167,7 @@
         <v>17.573526169063584</v>
       </c>
     </row>
-    <row r="78" spans="2:10">
+    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>116</v>
       </c>
@@ -7935,7 +8203,7 @@
         <v>17.408206949490399</v>
       </c>
     </row>
-    <row r="79" spans="2:10">
+    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>117</v>
       </c>
@@ -7971,7 +8239,7 @@
         <v>17.245911013237503</v>
       </c>
     </row>
-    <row r="80" spans="2:10">
+    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>118</v>
       </c>
@@ -8007,7 +8275,7 @@
         <v>17.086558555409884</v>
       </c>
     </row>
-    <row r="81" spans="2:10">
+    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>119</v>
       </c>
@@ -8043,7 +8311,7 @@
         <v>16.93007242516164</v>
       </c>
     </row>
-    <row r="82" spans="2:10">
+    <row r="82" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>120</v>
       </c>
@@ -8079,7 +8347,7 @@
         <v>16.776378025341472</v>
       </c>
     </row>
-    <row r="83" spans="2:10">
+    <row r="83" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>121</v>
       </c>
@@ -8123,12 +8391,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>